<commit_message>
removed FAST from title (for time being, hopefully)
</commit_message>
<xml_diff>
--- a/public/StructureDefinition-OAuthAuthenticationRequest.xlsx
+++ b/public/StructureDefinition-OAuthAuthenticationRequest.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="100">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-31T00:13:59-05:00</t>
+    <t>2023-04-11T09:52:12-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,13 +75,13 @@
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t>World</t>
+    <t>Global (Whole world)</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>This structure is defined to allow the FHIR Validator to validate a OAuthRegistration Response body</t>
+    <t>This structure defines an OAuth authentication response body</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -123,6 +123,9 @@
     <t>specialization</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>Path</t>
   </si>
   <si>
@@ -240,13 +243,17 @@
     <t>*</t>
   </si>
   <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
     <t>The response to the discovery endpoint</t>
   </si>
   <si>
     <t>Base</t>
   </si>
   <si>
-    <t>OAuthAuthenticationRequest.response_type</t>
+    <t>OAuthAuthenticationRequest.resourceType</t>
   </si>
   <si>
     <t>1</t>
@@ -256,13 +263,34 @@
 </t>
   </si>
   <si>
+    <t>Resource type</t>
+  </si>
+  <si>
+    <t>OAuthAuthenticationRequest.id</t>
+  </si>
+  <si>
+    <t>identifer</t>
+  </si>
+  <si>
+    <t>OAuthAuthenticationRequest.response-type</t>
+  </si>
+  <si>
+    <t>OAuthAuthenticationRequest.response_type</t>
+  </si>
+  <si>
     <t>Response code</t>
   </si>
   <si>
+    <t>OAuthAuthenticationRequest.client-id</t>
+  </si>
+  <si>
     <t>OAuthAuthenticationRequest.client_id</t>
   </si>
   <si>
     <t>Client ID</t>
+  </si>
+  <si>
+    <t>OAuthAuthenticationRequest.redirect-uri</t>
   </si>
   <si>
     <t>OAuthAuthenticationRequest.redirect_uri</t>
@@ -591,7 +619,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -600,42 +628,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.3515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.171875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.1484375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.06640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="40.37890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="40.234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="8.171875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.30859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.13671875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="14.21484375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="19.80078125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.60546875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="40.234375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="19.80078125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="17.60546875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="40.234375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.6796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="22.6796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -747,705 +775,935 @@
       <c r="AJ1" t="s" s="1">
         <v>71</v>
       </c>
+      <c r="AK1" t="s" s="1">
+        <v>72</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>73</v>
-      </c>
+      <c r="B2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
         <v>74</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="M2" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="M2" t="s" s="2">
+        <v>77</v>
+      </c>
       <c r="N2" s="2"/>
-      <c r="O2" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK2" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L3" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="M3" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="S3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="T3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="U3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="V3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="W3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Y3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Z3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AA3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF3" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="K3" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="R3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="S3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="T3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="U3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="V3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="W3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="X3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="Y3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="Z3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AA3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AB3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AC3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AD3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AE3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF3" t="s" s="2">
-        <v>78</v>
-      </c>
       <c r="AG3" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK3" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="F4" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="J4" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="K4" t="s" s="2">
-        <v>82</v>
-      </c>
       <c r="L4" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>84</v>
+      </c>
       <c r="N4" s="2"/>
-      <c r="O4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK4" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>87</v>
+      </c>
       <c r="N5" s="2"/>
-      <c r="O5" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK5" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="M6" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="M6" t="s" s="2">
+        <v>90</v>
+      </c>
       <c r="N6" s="2"/>
-      <c r="O6" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK6" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="M7" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N7" s="2"/>
-      <c r="O7" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q7" s="2"/>
       <c r="R7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK7" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="M8" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="M8" t="s" s="2">
+        <v>95</v>
+      </c>
       <c r="N8" s="2"/>
-      <c r="O8" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" t="s" s="2">
-        <v>72</v>
-      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AK8" t="s" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K9" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="M9" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="S9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="T9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="U9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="V9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="W9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Y9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Z9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AA9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF9" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AG9" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH9" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AK9" t="s" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="M10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="S10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="T10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="U10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="V10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="W10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Y10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Z10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AA10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF10" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AG10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ10" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AK10" t="s" s="2">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>